<commit_message>
add working deleteLastEntry button
</commit_message>
<xml_diff>
--- a/invenageConf.xlsx
+++ b/invenageConf.xlsx
@@ -6,7 +6,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/umdocc/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/umdocc/Dropbox/Invenage/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="35">
   <si>
     <t>Name</t>
   </si>
@@ -75,9 +75,6 @@
     <t>Vi</t>
   </si>
   <si>
-    <t>masterDataPath</t>
-  </si>
-  <si>
     <t>slaveDataPath</t>
   </si>
   <si>
@@ -112,6 +109,30 @@
   </si>
   <si>
     <t>Dropbox/MDSTrungThien/Shared/POReview</t>
+  </si>
+  <si>
+    <t>databasePath</t>
+  </si>
+  <si>
+    <t>Dropbox/MDSTrungThien/Shared/Invenage.sqlite</t>
+  </si>
+  <si>
+    <t>dbType</t>
+  </si>
+  <si>
+    <t>SQLite</t>
+  </si>
+  <si>
+    <t>sqlUserName</t>
+  </si>
+  <si>
+    <t>sqlPassword</t>
+  </si>
+  <si>
+    <t>umdocc</t>
+  </si>
+  <si>
+    <t>mdstrungthien</t>
   </si>
 </sst>
 </file>
@@ -426,10 +447,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -439,7 +460,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -450,7 +471,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C2" t="s">
         <v>3</v>
@@ -458,123 +479,156 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>15</v>
+        <v>29</v>
       </c>
       <c r="B3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C3" t="s">
-        <v>20</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>27</v>
       </c>
       <c r="B4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C4" t="s">
-        <v>5</v>
+        <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>31</v>
       </c>
       <c r="B5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C5" t="s">
-        <v>24</v>
+        <v>33</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>7</v>
+        <v>32</v>
       </c>
       <c r="B6" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C6" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="B7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C7" t="s">
-        <v>20</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C8" t="s">
-        <v>9</v>
+        <v>23</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C9" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="B10" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" t="s">
         <v>19</v>
-      </c>
-      <c r="C10" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B11" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C11" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C12" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13" t="s">
+        <v>18</v>
+      </c>
+      <c r="C13" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14" t="s">
+        <v>20</v>
+      </c>
+      <c r="C14" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>13</v>
+      </c>
+      <c r="B15" t="s">
+        <v>20</v>
+      </c>
+      <c r="C15" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>21</v>
+      </c>
+      <c r="B16" t="s">
+        <v>20</v>
+      </c>
+      <c r="C16" t="s">
         <v>22</v>
-      </c>
-      <c r="B13" t="s">
-        <v>21</v>
-      </c>
-      <c r="C13" t="s">
-        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>